<commit_message>
move requires into rastera.analytical
</commit_message>
<xml_diff>
--- a/Axcels/beautiful.xlsx
+++ b/Axcels/beautiful.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="10680" tabRatio="885" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="24780" windowHeight="11040" tabRatio="885" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="rate" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156">
   <si>
     <t>abbr</t>
   </si>
@@ -500,23 +500,10 @@
     <t>Requires:Sound.wav mp3  wave hash combine water decipher</t>
   </si>
   <si>
-    <t>红胖子(红模仿)的博文大全：开发技术集合（包含Qt实用技术、树莓派、三维、OpenCV、OpenGL、ffmpeg、OSG、单片机、软硬结合等等）持续更新中…（点击传送门）</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An.dev 需求理序概括
-txt md html
-md.isapped.false
-    md.uml.kansai.first
-    md.table.user
-html.jquery.vue
-    html.user.form.svg.rect.table.flex
-kolor with one Upperlower
-全部操作系统 最底层TXT开始
-symbolmetrik kof alloic metricwitch first
-其他语言 metric~index
-结构设计:分隔符 文字 belongto ，
-立体 求 balance necklace
-</t>
+    <t>树莓派、三维、OpenCV、OpenGL、ffmpeg、OSG、单片机</t>
+  </si>
+  <si>
+    <t>Flat.Colorful.KidFist.AxisLine|Flat.Design</t>
   </si>
   <si>
     <t>parent_id</t>
@@ -596,10 +583,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -632,6 +619,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -639,15 +648,75 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -662,20 +731,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -683,77 +738,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -768,10 +755,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -815,6 +802,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -827,18 +868,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -851,151 +982,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,11 +998,63 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1039,70 +1078,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1111,160 +1098,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1284,54 +1268,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1627,7 +1611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -1635,217 +1619,217 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="2" width="9" style="4"/>
-    <col min="3" max="3" width="24.8761061946903" style="4" customWidth="1"/>
-    <col min="4" max="4" width="61.8761061946903" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.8761061946903" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.2477876106195" style="4" customWidth="1"/>
-    <col min="7" max="7" width="19.1238938053097" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="4"/>
+    <col min="1" max="2" width="9" style="3"/>
+    <col min="3" max="3" width="24.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="61.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.6</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f>1-F2</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.4</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f>1-F3</f>
         <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f>1-F4</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="17" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.05</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.05</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f>1-F5</f>
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="17" spans="1:7">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.01</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.01</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f>1-F6</f>
         <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="G7" s="4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
         <v>3.74</v>
       </c>
     </row>
     <row r="8" ht="90" customHeight="1" spans="1:5">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1856,336 +1840,336 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="9.3716814159292" style="4" customWidth="1"/>
-    <col min="3" max="3" width="44.8761061946903" style="4" customWidth="1"/>
-    <col min="4" max="4" width="80.5044247787611" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.6283185840708" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="9" style="3"/>
+    <col min="2" max="2" width="9.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="3:3">
-      <c r="C11" s="7"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>3</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>15</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>4</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>9</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>9</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>9</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>9</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" ht="38" customHeight="1" spans="1:4">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>9</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>9</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>9</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>9</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2197,7 +2181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A2:G15"/>
   <sheetViews>
@@ -2205,12 +2189,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="8.87610619469027" customWidth="1"/>
-    <col min="2" max="2" width="16.8761061946903" customWidth="1"/>
-    <col min="3" max="3" width="18.1238938053097" customWidth="1"/>
-    <col min="4" max="4" width="24.1238938053097" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
@@ -2302,225 +2286,225 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="2" width="9" style="4"/>
-    <col min="3" max="3" width="24.8761061946903" style="4" customWidth="1"/>
-    <col min="4" max="4" width="61.8761061946903" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.8761061946903" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.2477876106195" style="4" customWidth="1"/>
-    <col min="7" max="7" width="19.1238938053097" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="4"/>
+    <col min="1" max="2" width="9" style="3"/>
+    <col min="3" max="3" width="24.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="61.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:7">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="3" customFormat="1" spans="1:7">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="1" spans="1:7">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="3" customFormat="1" spans="1:7">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.6</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f t="shared" ref="G2:G6" si="0">1-F2</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="1" spans="1:7">
-      <c r="A3" s="5" t="s">
+    <row r="3" s="3" customFormat="1" spans="1:7">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.4</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="1" spans="1:7">
-      <c r="A4" s="5" t="s">
+    <row r="4" s="3" customFormat="1" spans="1:7">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="1" spans="1:7">
-      <c r="A5" s="5" t="s">
+    <row r="5" s="3" customFormat="1" ht="17" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.05</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.05</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" spans="1:7">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="3" customFormat="1" ht="17" spans="1:7">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.01</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.01</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" s="4" customFormat="1" spans="1:7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="G7" s="4">
+    <row r="7" s="3" customFormat="1" spans="1:7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
         <v>3.74</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="1" ht="90" customHeight="1" spans="1:5">
-      <c r="A8" s="5" t="s">
+    <row r="8" s="3" customFormat="1" ht="90" customHeight="1" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1" spans="1:5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+    <row r="9" s="3" customFormat="1" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1" spans="1:5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+    <row r="10" s="3" customFormat="1" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" s="4" customFormat="1" spans="1:5">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" s="3" customFormat="1" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" s="4" customFormat="1" spans="1:5">
-      <c r="A12" s="4" t="s">
+    <row r="12" s="3" customFormat="1" spans="1:5">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2531,18 +2515,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="38.2477876106195" customWidth="1"/>
-    <col min="2" max="2" width="68.2477876106195" customWidth="1"/>
+    <col min="1" max="1" width="38.25" customWidth="1"/>
+    <col min="2" max="2" width="68.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2745,18 +2729,18 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" ht="17" spans="2:2">
       <c r="B29" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" ht="229.5" spans="2:2">
-      <c r="B31" s="3" t="s">
+    <row r="31" ht="17" spans="2:2">
+      <c r="B31" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2767,7 +2751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -2775,12 +2759,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="4" max="4" width="23.2477876106195" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="22.2477876106195" customWidth="1"/>
-    <col min="9" max="9" width="10.3716814159292" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2895,7 +2879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A2:A3"/>
   <sheetViews>
@@ -2903,9 +2887,9 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="28.2477876106195" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">

</xml_diff>